<commit_message>
add map and multiset data type cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="718">
   <si>
     <t>TestID</t>
   </si>
@@ -900,151 +900,6 @@
     <t>select * from $partition48</t>
   </si>
   <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_01.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_02.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_03.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_04.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_05.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_06.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_07.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_08.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_09.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_10.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_11.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_12.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_13.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_14.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_15.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_16.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_17.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_18.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_19.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_20.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_21.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_22.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_23.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_24.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_25.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_26.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_27.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_28.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_29.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_30.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_31.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_32.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_33.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_34.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_35.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_36.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_37.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_38.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_39.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_40.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_41.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_42.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_43.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_44.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_45.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_46.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_47.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition_48.csv</t>
-  </si>
-  <si>
     <t>创建分区表，整型主键单分区值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1525,10 +1380,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/array_001.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>创建表，数组类型列位于表首列，主键在中间列</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1547,9 +1398,6 @@
     <t>select * from $array20</t>
   </si>
   <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/array_002.csv</t>
-  </si>
-  <si>
     <t>select name,age,class_no,amount,id from $array19</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1577,9 +1425,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/array_003.csv</t>
-  </si>
-  <si>
     <t>array_04</t>
   </si>
   <si>
@@ -1595,7 +1440,1039 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/array_004.csv</t>
+    <t>map_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定map字段插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map1_value11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $map1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map_02</t>
+  </si>
+  <si>
+    <t>map字段允许为null,不指定map字段插入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map1_value12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map_03</t>
+  </si>
+  <si>
+    <t>向有map默认值的表插入数据，指定字段不含map类型字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map3_value15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $map3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map_04</t>
+  </si>
+  <si>
+    <t>Map在中间列插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map4</t>
+  </si>
+  <si>
+    <t>map4_value16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $map4</t>
+  </si>
+  <si>
+    <t>map_05</t>
+  </si>
+  <si>
+    <t>Map在首列插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map5</t>
+  </si>
+  <si>
+    <t>map5_value17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $map5</t>
+  </si>
+  <si>
+    <t>map_06</t>
+  </si>
+  <si>
+    <t>Map不同类型key值插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map1_value19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $map1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset_02</t>
+  </si>
+  <si>
+    <t>multiset_03</t>
+  </si>
+  <si>
+    <t>multiset_04</t>
+  </si>
+  <si>
+    <t>multiset_05</t>
+  </si>
+  <si>
+    <t>multiset_06</t>
+  </si>
+  <si>
+    <t>multiset_07</t>
+  </si>
+  <si>
+    <t>multiset_08</t>
+  </si>
+  <si>
+    <t>multiset_09</t>
+  </si>
+  <si>
+    <t>Multiset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset12</t>
+  </si>
+  <si>
+    <t>multiset13</t>
+  </si>
+  <si>
+    <t>multiset14</t>
+  </si>
+  <si>
+    <t>multiset15</t>
+  </si>
+  <si>
+    <t>multiset16</t>
+  </si>
+  <si>
+    <t>multiset17</t>
+  </si>
+  <si>
+    <t>multiset11_value11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset12_value12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset13_value13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset14_value14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset15_value15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset16_value16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset17_value17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset12</t>
+  </si>
+  <si>
+    <t>select * from $multiset13</t>
+  </si>
+  <si>
+    <t>select * from $multiset14</t>
+  </si>
+  <si>
+    <t>select * from $multiset15</t>
+  </si>
+  <si>
+    <t>select * from $multiset16</t>
+  </si>
+  <si>
+    <t>select * from $multiset17</t>
+  </si>
+  <si>
+    <t>Multiset在中间列插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multiset在首列插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向有int multiset默认值的表插入数据，指定字段不含multiset类型字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向有varchar multiset默认值的表插入数据，指定字段不含multiset类型字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向有double multiset默认值的表插入数据，指定字段不含multiset类型字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向有date multiset默认值的表插入数据，指定字段不含multiset类型字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向有time multiset默认值的表插入数据，指定字段不含multiset类型字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向有timestamp multiset默认值的表插入数据，指定字段不含multiset类型字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向有boolean multiset默认值的表插入数据，指定字段不含multiset类型字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset18</t>
+  </si>
+  <si>
+    <t>multiset19</t>
+  </si>
+  <si>
+    <t>multiset18_value18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset19_value19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset18</t>
+  </si>
+  <si>
+    <t>select * from $multiset19</t>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset_10</t>
+  </si>
+  <si>
+    <t>multiset_11</t>
+  </si>
+  <si>
+    <t>Int multiset列值为null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset1_value20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varchar multiset列值为null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset_12</t>
+  </si>
+  <si>
+    <t>multiset_13</t>
+  </si>
+  <si>
+    <t>multiset_14</t>
+  </si>
+  <si>
+    <t>multiset_15</t>
+  </si>
+  <si>
+    <t>multiset_16</t>
+  </si>
+  <si>
+    <t>multiset_17</t>
+  </si>
+  <si>
+    <t>multiset_18</t>
+  </si>
+  <si>
+    <t>multiset_19</t>
+  </si>
+  <si>
+    <t>multiset_20</t>
+  </si>
+  <si>
+    <t>multiset_21</t>
+  </si>
+  <si>
+    <t>multiset_22</t>
+  </si>
+  <si>
+    <t>multiset_23</t>
+  </si>
+  <si>
+    <t>multiset_24</t>
+  </si>
+  <si>
+    <t>multiset_25</t>
+  </si>
+  <si>
+    <t>multiset_26</t>
+  </si>
+  <si>
+    <t>multiset_27</t>
+  </si>
+  <si>
+    <t>multiset_28</t>
+  </si>
+  <si>
+    <t>multiset_29</t>
+  </si>
+  <si>
+    <t>multiset_30</t>
+  </si>
+  <si>
+    <t>multiset_31</t>
+  </si>
+  <si>
+    <t>multiset_32</t>
+  </si>
+  <si>
+    <t>multiset_33</t>
+  </si>
+  <si>
+    <t>multiset_34</t>
+  </si>
+  <si>
+    <t>multiset_35</t>
+  </si>
+  <si>
+    <t>multiset_36</t>
+  </si>
+  <si>
+    <t>Multiset插入混合类型元素成功</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset1_value22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset3</t>
+  </si>
+  <si>
+    <t>select * from $multiset5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset5_value23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date型multiset对不同日期格式的支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset7_value25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time型multiset对不同日期格式的支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset8</t>
+  </si>
+  <si>
+    <t>multiset8_value26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset8</t>
+  </si>
+  <si>
+    <t>Timestamp型multiset对不同日期格式的支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset9</t>
+  </si>
+  <si>
+    <t>multiset9_value27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset9</t>
+  </si>
+  <si>
+    <t>Int multiset插入多条数据，元素均为浮点数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Int multiset插入多条数据，元素均为数值字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Int multiset插入多条数据，元素均为布尔值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset1_value28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset1_value29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset1_value30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varchar multiset插入多条数据，元素均为整数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varchar multiset插入多条数据，元素均为浮点数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varchar multiset插入多条数据，元素均为布尔值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varchar multiset插入多条数据，元素均为日期字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varchar multiset插入多条数据，元素均为时间字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varchar multiset插入多条数据，元素均为日期时间字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double multiset插入多条数据，元素均为整数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double multiset插入多条数据，元素均为数值字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double multiset插入多条数据，元素均为布尔值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset5_value38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset5_value39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset5_value40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varchar multiset插入数据，元素均为整型和浮点数混合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timestamp multiset插入数据，元素均为整数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset9_value41</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset9_value42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boolean multiset插入数据，元素均为整数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset10</t>
+  </si>
+  <si>
+    <t>multiset10_value43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset10</t>
+  </si>
+  <si>
+    <t>Varchar multiset插入空字符串元素和重复元素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value46</t>
+  </si>
+  <si>
+    <t>multiset1_value45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Int multiset插入元素个数较多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varchar multiset插入元素个数较多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_01.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_02.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_03.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_04.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_05.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_06.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_07.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_08.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_09.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_10.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_11.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_12.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_13.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_14.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_15.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_16.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_17.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_18.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_19.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_20.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_21.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_22.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_23.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_24.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_25.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_26.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_27.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_28.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_29.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_30.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_31.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_32.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_33.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_34.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_35.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_36.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_37.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_38.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_39.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_40.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_41.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_42.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_43.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_44.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_45.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_46.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_47.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/partition/partition_48.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/array/array_001.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/array/array_002.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/array/array_003.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/array/array_004.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/map/map_001.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/map/map_002.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/map/map_003.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/map/map_004.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/map/map_005.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/map/map_006.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset001.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset002.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset003.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset004.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset005.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset006.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset007.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset008.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset009.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset010.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset011.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset012.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset013.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset014.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset015.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset016.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset017.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset018.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset019.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset020.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset021.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset022.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset023.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset024.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset025.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset026.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset027.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset028.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset029.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset030.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset031.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset032.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset033.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset034.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset035.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset036.csv</t>
+  </si>
+  <si>
+    <t>multiset_37</t>
+  </si>
+  <si>
+    <t>创建含有多个multiset字段表并插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $multiset20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset037.csv</t>
+  </si>
+  <si>
+    <t>multiset20_value47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset_38</t>
+  </si>
+  <si>
+    <t>multiset字段允许为Null, 不指定multiset字段插入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset038.csv</t>
+  </si>
+  <si>
+    <t>multiset_39</t>
+  </si>
+  <si>
+    <t>指定multiset字段插入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiset3_value50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/multiset/multiset039.csv</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -1972,24 +2849,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39.375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="17.875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="19.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="10.75" style="9" customWidth="1"/>
     <col min="12" max="12" width="20.25" style="7" customWidth="1"/>
     <col min="13" max="13" width="12" style="1" bestFit="1" customWidth="1"/>
@@ -2072,6 +2949,7 @@
       <c r="J2" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="O2" s="6" t="s">
@@ -2106,6 +2984,7 @@
       <c r="J3" s="9" t="s">
         <v>24</v>
       </c>
+      <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="7"/>
       <c r="O3" s="6" t="s">
@@ -2184,6 +3063,7 @@
       <c r="J5" s="9" t="s">
         <v>48</v>
       </c>
+      <c r="K5" s="3"/>
       <c r="O5" s="1" t="s">
         <v>10</v>
       </c>
@@ -2216,6 +3096,7 @@
       <c r="J6" s="9" t="s">
         <v>49</v>
       </c>
+      <c r="K6" s="3"/>
       <c r="O6" s="7" t="s">
         <v>10</v>
       </c>
@@ -2248,6 +3129,7 @@
       <c r="J7" s="9" t="s">
         <v>50</v>
       </c>
+      <c r="K7" s="3"/>
       <c r="O7" s="7" t="s">
         <v>10</v>
       </c>
@@ -2324,6 +3206,7 @@
       <c r="J9" s="9" t="s">
         <v>82</v>
       </c>
+      <c r="K9" s="3"/>
       <c r="O9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2357,6 +3240,7 @@
       <c r="J10" s="9" t="s">
         <v>85</v>
       </c>
+      <c r="K10" s="3"/>
       <c r="O10" s="1" t="s">
         <v>10</v>
       </c>
@@ -2390,6 +3274,7 @@
       <c r="J11" s="9" t="s">
         <v>94</v>
       </c>
+      <c r="K11" s="3"/>
       <c r="O11" s="7" t="s">
         <v>10</v>
       </c>
@@ -2423,6 +3308,7 @@
       <c r="J12" s="9" t="s">
         <v>103</v>
       </c>
+      <c r="K12" s="3"/>
       <c r="O12" s="7" t="s">
         <v>10</v>
       </c>
@@ -2456,6 +3342,7 @@
       <c r="J13" s="9" t="s">
         <v>104</v>
       </c>
+      <c r="K13" s="3"/>
       <c r="O13" s="7" t="s">
         <v>10</v>
       </c>
@@ -2489,6 +3376,7 @@
       <c r="J14" s="9" t="s">
         <v>110</v>
       </c>
+      <c r="K14" s="3"/>
       <c r="O14" s="7" t="s">
         <v>10</v>
       </c>
@@ -2522,6 +3410,7 @@
       <c r="J15" s="9" t="s">
         <v>117</v>
       </c>
+      <c r="K15" s="3"/>
       <c r="O15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2554,19 +3443,20 @@
       <c r="J16" s="9" t="s">
         <v>124</v>
       </c>
+      <c r="K16" s="3"/>
       <c r="O16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>389</v>
+        <v>341</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>318</v>
+        <v>270</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>125</v>
@@ -2578,27 +3468,28 @@
         <v>174</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>320</v>
+        <v>272</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>222</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>270</v>
-      </c>
+        <v>606</v>
+      </c>
+      <c r="K17" s="3"/>
       <c r="O17" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>390</v>
+        <v>342</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>319</v>
+        <v>271</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>125</v>
@@ -2610,27 +3501,28 @@
         <v>175</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>223</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>271</v>
-      </c>
+        <v>607</v>
+      </c>
+      <c r="K18" s="3"/>
       <c r="O18" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>391</v>
+        <v>343</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>322</v>
+        <v>274</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>125</v>
@@ -2642,27 +3534,28 @@
         <v>176</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>224</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>272</v>
-      </c>
+        <v>608</v>
+      </c>
+      <c r="K19" s="3"/>
       <c r="O19" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>392</v>
+        <v>344</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>324</v>
+        <v>276</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>125</v>
@@ -2674,27 +3567,28 @@
         <v>177</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>225</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>273</v>
-      </c>
+        <v>609</v>
+      </c>
+      <c r="K20" s="3"/>
       <c r="O20" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>393</v>
+        <v>345</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>125</v>
@@ -2706,27 +3600,28 @@
         <v>178</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>226</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>274</v>
-      </c>
+        <v>610</v>
+      </c>
+      <c r="K21" s="3"/>
       <c r="O21" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>394</v>
+        <v>346</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>327</v>
+        <v>279</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>125</v>
@@ -2738,27 +3633,28 @@
         <v>179</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>227</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>275</v>
-      </c>
+        <v>611</v>
+      </c>
+      <c r="K22" s="3"/>
       <c r="O22" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
-        <v>395</v>
+        <v>347</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>330</v>
+        <v>282</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>125</v>
@@ -2770,27 +3666,28 @@
         <v>180</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>228</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>276</v>
-      </c>
+        <v>612</v>
+      </c>
+      <c r="K23" s="3"/>
       <c r="O23" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="7" t="s">
-        <v>396</v>
+        <v>348</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>331</v>
+        <v>283</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>125</v>
@@ -2802,27 +3699,28 @@
         <v>181</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>229</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>277</v>
-      </c>
+        <v>613</v>
+      </c>
+      <c r="K24" s="3"/>
       <c r="O24" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
-        <v>397</v>
+        <v>349</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>332</v>
+        <v>284</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>125</v>
@@ -2834,27 +3732,28 @@
         <v>182</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>230</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>278</v>
-      </c>
+        <v>614</v>
+      </c>
+      <c r="K25" s="3"/>
       <c r="O25" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
-        <v>398</v>
+        <v>350</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>333</v>
+        <v>285</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>125</v>
@@ -2866,27 +3765,28 @@
         <v>183</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>231</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>279</v>
-      </c>
+        <v>615</v>
+      </c>
+      <c r="K26" s="3"/>
       <c r="O26" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
-        <v>399</v>
+        <v>351</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>125</v>
@@ -2898,27 +3798,28 @@
         <v>184</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>232</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>280</v>
-      </c>
+        <v>616</v>
+      </c>
+      <c r="K27" s="3"/>
       <c r="O27" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>400</v>
+        <v>352</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>335</v>
+        <v>287</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>125</v>
@@ -2930,27 +3831,28 @@
         <v>185</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>337</v>
+        <v>289</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>233</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>281</v>
-      </c>
+        <v>617</v>
+      </c>
+      <c r="K28" s="3"/>
       <c r="O28" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
-        <v>401</v>
+        <v>353</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>336</v>
+        <v>288</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>125</v>
@@ -2962,27 +3864,28 @@
         <v>186</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>234</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>282</v>
-      </c>
+        <v>618</v>
+      </c>
+      <c r="K29" s="3"/>
       <c r="O29" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>402</v>
+        <v>354</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>338</v>
+        <v>290</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>125</v>
@@ -2994,27 +3897,28 @@
         <v>187</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>337</v>
+        <v>289</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>235</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>283</v>
-      </c>
+        <v>619</v>
+      </c>
+      <c r="K30" s="3"/>
       <c r="O30" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
-        <v>403</v>
+        <v>355</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>339</v>
+        <v>291</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>125</v>
@@ -3026,27 +3930,28 @@
         <v>188</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>342</v>
+        <v>294</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>236</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>284</v>
-      </c>
+        <v>620</v>
+      </c>
+      <c r="K31" s="3"/>
       <c r="O31" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
-        <v>404</v>
+        <v>356</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>340</v>
+        <v>292</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>125</v>
@@ -3058,27 +3963,28 @@
         <v>189</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>337</v>
+        <v>289</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>237</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>285</v>
-      </c>
+        <v>621</v>
+      </c>
+      <c r="K32" s="3"/>
       <c r="O32" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
-        <v>405</v>
+        <v>357</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>341</v>
+        <v>293</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>125</v>
@@ -3090,27 +3996,28 @@
         <v>190</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>238</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>286</v>
-      </c>
+        <v>622</v>
+      </c>
+      <c r="K33" s="3"/>
       <c r="O33" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
-        <v>406</v>
+        <v>358</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>343</v>
+        <v>295</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>125</v>
@@ -3122,27 +4029,28 @@
         <v>191</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>239</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>287</v>
-      </c>
+        <v>623</v>
+      </c>
+      <c r="K34" s="3"/>
       <c r="O34" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
-        <v>407</v>
+        <v>359</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>344</v>
+        <v>296</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>125</v>
@@ -3154,27 +4062,28 @@
         <v>192</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>240</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>288</v>
-      </c>
+        <v>624</v>
+      </c>
+      <c r="K35" s="3"/>
       <c r="O35" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
-        <v>408</v>
+        <v>360</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>348</v>
+        <v>300</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>125</v>
@@ -3186,27 +4095,28 @@
         <v>193</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>346</v>
+        <v>298</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>241</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>289</v>
-      </c>
+        <v>625</v>
+      </c>
+      <c r="K36" s="3"/>
       <c r="O36" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
-        <v>409</v>
+        <v>361</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>347</v>
+        <v>299</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>125</v>
@@ -3218,27 +4128,28 @@
         <v>194</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>349</v>
+        <v>301</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>242</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>290</v>
-      </c>
+        <v>626</v>
+      </c>
+      <c r="K37" s="3"/>
       <c r="O37" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
-        <v>410</v>
+        <v>362</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>350</v>
+        <v>302</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>125</v>
@@ -3250,27 +4161,28 @@
         <v>195</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>243</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>291</v>
-      </c>
+        <v>627</v>
+      </c>
+      <c r="K38" s="3"/>
       <c r="O38" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39" s="7" t="s">
-        <v>411</v>
+        <v>363</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>351</v>
+        <v>303</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>125</v>
@@ -3282,27 +4194,28 @@
         <v>196</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>244</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>628</v>
+      </c>
+      <c r="K39" s="3"/>
       <c r="O39" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A40" s="7" t="s">
-        <v>412</v>
+        <v>364</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>125</v>
@@ -3314,27 +4227,28 @@
         <v>197</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>245</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>293</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="K40" s="3"/>
       <c r="O40" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41" s="7" t="s">
-        <v>413</v>
+        <v>365</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>355</v>
+        <v>307</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>125</v>
@@ -3346,27 +4260,28 @@
         <v>198</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>320</v>
+        <v>272</v>
       </c>
       <c r="I41" s="3" t="s">
         <v>246</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>294</v>
-      </c>
+        <v>630</v>
+      </c>
+      <c r="K41" s="3"/>
       <c r="O41" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
-        <v>414</v>
+        <v>366</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>356</v>
+        <v>308</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>125</v>
@@ -3378,27 +4293,28 @@
         <v>199</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>357</v>
+        <v>309</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>247</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>295</v>
-      </c>
+        <v>631</v>
+      </c>
+      <c r="K42" s="3"/>
       <c r="O42" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
-        <v>415</v>
+        <v>367</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>358</v>
+        <v>310</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>125</v>
@@ -3410,27 +4326,28 @@
         <v>200</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>248</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>296</v>
-      </c>
+        <v>632</v>
+      </c>
+      <c r="K43" s="3"/>
       <c r="O43" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
-        <v>416</v>
+        <v>368</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>359</v>
+        <v>311</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>125</v>
@@ -3442,27 +4359,28 @@
         <v>201</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>249</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>297</v>
-      </c>
+        <v>633</v>
+      </c>
+      <c r="K44" s="3"/>
       <c r="O44" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A45" s="7" t="s">
-        <v>417</v>
+        <v>369</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>360</v>
+        <v>312</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>125</v>
@@ -3474,27 +4392,28 @@
         <v>202</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>250</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>298</v>
-      </c>
+        <v>634</v>
+      </c>
+      <c r="K45" s="3"/>
       <c r="O45" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
-        <v>418</v>
+        <v>370</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>125</v>
@@ -3506,27 +4425,28 @@
         <v>203</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>362</v>
+        <v>314</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>251</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>299</v>
-      </c>
+        <v>635</v>
+      </c>
+      <c r="K46" s="3"/>
       <c r="O46" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47" s="7" t="s">
-        <v>419</v>
+        <v>371</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>363</v>
+        <v>315</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>125</v>
@@ -3538,27 +4458,28 @@
         <v>204</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>252</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>300</v>
-      </c>
+        <v>636</v>
+      </c>
+      <c r="K47" s="3"/>
       <c r="O47" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A48" s="7" t="s">
-        <v>420</v>
+        <v>372</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>364</v>
+        <v>316</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>125</v>
@@ -3570,27 +4491,28 @@
         <v>205</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>253</v>
       </c>
       <c r="J48" s="9" t="s">
-        <v>301</v>
-      </c>
+        <v>637</v>
+      </c>
+      <c r="K48" s="3"/>
       <c r="O48" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49" s="7" t="s">
-        <v>421</v>
+        <v>373</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>365</v>
+        <v>317</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>125</v>
@@ -3602,27 +4524,28 @@
         <v>206</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>366</v>
+        <v>318</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>254</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>302</v>
-      </c>
+        <v>638</v>
+      </c>
+      <c r="K49" s="3"/>
       <c r="O49" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
-        <v>422</v>
+        <v>374</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>367</v>
+        <v>319</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>125</v>
@@ -3634,27 +4557,28 @@
         <v>207</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>368</v>
+        <v>320</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>255</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>303</v>
-      </c>
+        <v>639</v>
+      </c>
+      <c r="K50" s="3"/>
       <c r="O50" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
-        <v>423</v>
+        <v>375</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>369</v>
+        <v>321</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>125</v>
@@ -3666,27 +4590,28 @@
         <v>208</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>372</v>
+        <v>324</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>256</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>304</v>
-      </c>
+        <v>640</v>
+      </c>
+      <c r="K51" s="3"/>
       <c r="O51" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52" s="7" t="s">
-        <v>424</v>
+        <v>376</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>370</v>
+        <v>322</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>125</v>
@@ -3698,27 +4623,28 @@
         <v>209</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>257</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>305</v>
-      </c>
+        <v>641</v>
+      </c>
+      <c r="K52" s="3"/>
       <c r="O52" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53" s="7" t="s">
-        <v>425</v>
+        <v>377</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>371</v>
+        <v>323</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>125</v>
@@ -3730,27 +4656,28 @@
         <v>210</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>372</v>
+        <v>324</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>258</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>306</v>
-      </c>
+        <v>642</v>
+      </c>
+      <c r="K53" s="3"/>
       <c r="O53" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54" s="7" t="s">
-        <v>426</v>
+        <v>378</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>373</v>
+        <v>325</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>125</v>
@@ -3762,27 +4689,28 @@
         <v>211</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>259</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>307</v>
-      </c>
+        <v>643</v>
+      </c>
+      <c r="K54" s="3"/>
       <c r="O54" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A55" s="7" t="s">
-        <v>427</v>
+        <v>379</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>374</v>
+        <v>326</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>125</v>
@@ -3794,27 +4722,28 @@
         <v>212</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>375</v>
+        <v>327</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>260</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>308</v>
-      </c>
+        <v>644</v>
+      </c>
+      <c r="K55" s="3"/>
       <c r="O55" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56" s="7" t="s">
-        <v>428</v>
+        <v>380</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>376</v>
+        <v>328</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>125</v>
@@ -3826,27 +4755,28 @@
         <v>213</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>377</v>
+        <v>329</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>261</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>309</v>
-      </c>
+        <v>645</v>
+      </c>
+      <c r="K56" s="3"/>
       <c r="O56" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
-        <v>429</v>
+        <v>381</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>378</v>
+        <v>330</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>125</v>
@@ -3858,27 +4788,28 @@
         <v>214</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>262</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>310</v>
-      </c>
+        <v>646</v>
+      </c>
+      <c r="K57" s="3"/>
       <c r="O57" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
-        <v>430</v>
+        <v>382</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>379</v>
+        <v>331</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>125</v>
@@ -3890,27 +4821,28 @@
         <v>215</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>263</v>
       </c>
       <c r="J58" s="9" t="s">
-        <v>311</v>
-      </c>
+        <v>647</v>
+      </c>
+      <c r="K58" s="3"/>
       <c r="O58" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
-        <v>431</v>
+        <v>383</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>380</v>
+        <v>332</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>125</v>
@@ -3922,27 +4854,28 @@
         <v>216</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>320</v>
+        <v>272</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>264</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>312</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="K59" s="3"/>
       <c r="O59" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A60" s="7" t="s">
-        <v>432</v>
+        <v>384</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>381</v>
+        <v>333</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>125</v>
@@ -3954,27 +4887,28 @@
         <v>217</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>346</v>
+        <v>298</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>265</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>313</v>
-      </c>
+        <v>649</v>
+      </c>
+      <c r="K60" s="3"/>
       <c r="O60" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A61" s="7" t="s">
-        <v>433</v>
+        <v>385</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>382</v>
+        <v>334</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>125</v>
@@ -3986,27 +4920,28 @@
         <v>218</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>266</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>314</v>
-      </c>
+        <v>650</v>
+      </c>
+      <c r="K61" s="3"/>
       <c r="O61" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A62" s="7" t="s">
-        <v>434</v>
+        <v>386</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>383</v>
+        <v>335</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>125</v>
@@ -4018,27 +4953,28 @@
         <v>219</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>368</v>
+        <v>320</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>267</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>315</v>
-      </c>
+        <v>651</v>
+      </c>
+      <c r="K62" s="3"/>
       <c r="O62" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A63" s="7" t="s">
-        <v>435</v>
+        <v>387</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>384</v>
+        <v>336</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>125</v>
@@ -4050,27 +4986,28 @@
         <v>220</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>268</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>316</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="K63" s="3"/>
       <c r="O63" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A64" s="7" t="s">
-        <v>436</v>
+        <v>388</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>385</v>
+        <v>337</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>125</v>
@@ -4082,193 +5019,1847 @@
         <v>221</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>269</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>317</v>
-      </c>
+        <v>653</v>
+      </c>
+      <c r="K64" s="3"/>
       <c r="O64" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A65" s="7" t="s">
-        <v>438</v>
+        <v>390</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>386</v>
+        <v>338</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>388</v>
+        <v>340</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>440</v>
+        <v>392</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>437</v>
+        <v>389</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>387</v>
+        <v>339</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>441</v>
+        <v>393</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>439</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="K65" s="3"/>
       <c r="O65" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>442</v>
+        <v>394</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>8</v>
+        <v>717</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>444</v>
+        <v>396</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>445</v>
+        <v>397</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>446</v>
+        <v>398</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>447</v>
+        <v>399</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>448</v>
+        <v>400</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>449</v>
+        <v>401</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>457</v>
+        <v>407</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>450</v>
-      </c>
+        <v>654</v>
+      </c>
+      <c r="K66" s="3"/>
       <c r="O66" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A67" s="7" t="s">
-        <v>443</v>
+        <v>395</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>8</v>
+        <v>717</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>451</v>
+        <v>402</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>445</v>
+        <v>397</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>446</v>
+        <v>398</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>452</v>
+        <v>403</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>453</v>
+        <v>404</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>454</v>
+        <v>405</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>455</v>
+        <v>406</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>456</v>
-      </c>
+        <v>655</v>
+      </c>
+      <c r="K67" s="3"/>
       <c r="O67" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A68" s="7" t="s">
-        <v>458</v>
+        <v>408</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>8</v>
+        <v>717</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>459</v>
+        <v>409</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>445</v>
+        <v>397</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>446</v>
+        <v>398</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>460</v>
+        <v>410</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>462</v>
+        <v>412</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>461</v>
+        <v>411</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>463</v>
+        <v>413</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>464</v>
-      </c>
+        <v>656</v>
+      </c>
+      <c r="K68" s="3"/>
       <c r="O68" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A69" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="J69" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="K69" s="3"/>
+      <c r="O69" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A70" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="J70" s="9" t="s">
+        <v>658</v>
+      </c>
+      <c r="K70" s="3"/>
+      <c r="O70" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A71" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="J71" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="K71" s="3"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A72" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="J72" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="K72" s="3"/>
+      <c r="O72" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A73" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="J73" s="9" t="s">
+        <v>661</v>
+      </c>
+      <c r="K73" s="3"/>
+      <c r="O73" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A74" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="J74" s="9" t="s">
+        <v>662</v>
+      </c>
+      <c r="K74" s="3"/>
+      <c r="O74" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A75" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="J75" s="9" t="s">
+        <v>663</v>
+      </c>
+      <c r="K75" s="3"/>
+      <c r="O75" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="J76" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="K76" s="3"/>
+      <c r="O76" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A77" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="J77" s="9" t="s">
+        <v>665</v>
+      </c>
+      <c r="K77" s="3"/>
+      <c r="O77" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A78" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="J78" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="K78" s="3"/>
+      <c r="O78" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A79" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="J79" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="K79" s="3"/>
+      <c r="O79" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A80" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="G80" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="J80" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="K80" s="3"/>
+      <c r="O80" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A81" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F81" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="G81" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="J81" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="K81" s="3"/>
+      <c r="O81" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A82" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F82" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>460</v>
-      </c>
-      <c r="G69" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="J69" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="O69" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
+      <c r="G82" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="J82" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="K82" s="3"/>
+      <c r="O82" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A83" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="J83" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="K83" s="3"/>
+      <c r="O83" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A84" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="J84" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="K84" s="3"/>
+      <c r="O84" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A85" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="J85" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="K85" s="3"/>
+      <c r="O85" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A86" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="J86" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="K86" s="3"/>
+      <c r="O86" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A87" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="J87" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="K87" s="3"/>
+      <c r="O87" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A88" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="G88" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="J88" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="K88" s="3"/>
+      <c r="O88" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A89" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="J89" s="9" t="s">
+        <v>677</v>
+      </c>
+      <c r="K89" s="3"/>
+      <c r="O89" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A90" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="J90" s="9" t="s">
+        <v>678</v>
+      </c>
+      <c r="K90" s="3"/>
+      <c r="O90" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A91" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="J91" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="K91" s="3"/>
+      <c r="O91" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A92" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="J92" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="K92" s="3"/>
+      <c r="O92" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A93" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="J93" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="K93" s="3"/>
+      <c r="O93" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A94" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="G94" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="J94" s="9" t="s">
+        <v>682</v>
+      </c>
+      <c r="K94" s="3"/>
+      <c r="O94" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A95" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="J95" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="K95" s="3"/>
+      <c r="O95" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A96" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="J96" s="9" t="s">
+        <v>684</v>
+      </c>
+      <c r="K96" s="3"/>
+      <c r="O96" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A97" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="J97" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="K97" s="3"/>
+      <c r="O97" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A98" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G98" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="J98" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="K98" s="3"/>
+      <c r="O98" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A99" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="J99" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="K99" s="3"/>
+      <c r="O99" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A100" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G100" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="J100" s="9" t="s">
+        <v>688</v>
+      </c>
+      <c r="K100" s="3"/>
+      <c r="O100" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A101" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="J101" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="K101" s="3"/>
+      <c r="O101" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A102" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G102" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="J102" s="9" t="s">
+        <v>690</v>
+      </c>
+      <c r="K102" s="3"/>
+      <c r="O102" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A103" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="J103" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="K103" s="3"/>
+      <c r="O103" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A104" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="G104" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="J104" s="9" t="s">
+        <v>692</v>
+      </c>
+      <c r="K104" s="3"/>
+      <c r="O104" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A105" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="J105" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="K105" s="3"/>
+      <c r="O105" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A106" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="G106" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="J106" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="K106" s="3"/>
+      <c r="O106" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A107" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="J107" s="9" t="s">
+        <v>695</v>
+      </c>
+      <c r="K107" s="3"/>
+      <c r="O107" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A108" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="G108" s="7" t="s">
+        <v>596</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="J108" s="9" t="s">
+        <v>696</v>
+      </c>
+      <c r="K108" s="3"/>
+      <c r="O108" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A109" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="J109" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="K109" s="3"/>
+      <c r="O109" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A110" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="G110" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="J110" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="K110" s="3"/>
+      <c r="O110" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A111" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G111" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="J111" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="K111" s="3"/>
+      <c r="O111" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A112" s="7" t="s">
+        <v>700</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="G112" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="J112" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="K112" s="3"/>
+      <c r="O112" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A113" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="G113" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="J113" s="9" t="s">
+        <v>711</v>
+      </c>
+      <c r="K113" s="3"/>
+      <c r="O113" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A114" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="G114" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="J114" s="9" t="s">
+        <v>716</v>
+      </c>
+      <c r="K114" s="3"/>
+      <c r="O114" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K115" s="3"/>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K116" s="3"/>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K117" s="3"/>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K118" s="3"/>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K119" s="3"/>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K120" s="3"/>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K121" s="3"/>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K122" s="3"/>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K123" s="3"/>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K124" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add DML test for MySQL protocol
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
@@ -2851,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="C104" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add two insert cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="748">
   <si>
     <t>TestID</t>
   </si>
@@ -2517,6 +2517,60 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/insert_017.csv</t>
+  </si>
+  <si>
+    <t>insert_018</t>
+  </si>
+  <si>
+    <t>insert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_value15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/insert_018.csv</t>
+  </si>
+  <si>
+    <t>insert_019</t>
+  </si>
+  <si>
+    <t>指定非连续字段插入数据1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定非连续字段插入数据2</t>
+  </si>
+  <si>
+    <t>schema17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_value16</t>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/insert_019.csv</t>
   </si>
 </sst>
 </file>
@@ -2900,10 +2954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O116"/>
+  <dimension ref="A1:O118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6943,6 +6997,70 @@
         <v>732</v>
       </c>
       <c r="O116" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A117" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="J117" s="9" t="s">
+        <v>739</v>
+      </c>
+      <c r="O117" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A118" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="G118" s="7" t="s">
+        <v>744</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="J118" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="O118" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add case about create table with replica specified
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="776">
   <si>
     <t>TestID</t>
   </si>
@@ -2597,6 +2597,78 @@
   </si>
   <si>
     <t>select id from $autoinc2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_021</t>
+  </si>
+  <si>
+    <t>insert_022</t>
+  </si>
+  <si>
+    <t>指定replica为1,插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定replica为2,插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_023</t>
+  </si>
+  <si>
+    <t>指定replica为3,插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema29</t>
+  </si>
+  <si>
+    <t>schema30</t>
+  </si>
+  <si>
+    <t>insert_value18</t>
+  </si>
+  <si>
+    <t>insert_value17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_value19</t>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema29</t>
+  </si>
+  <si>
+    <t>select * from $schema30</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/insert_021.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/insert_022.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/insert_023.csv</t>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2981,10 +3053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O119"/>
+  <dimension ref="A1:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6967,7 +7039,7 @@
       <c r="A115" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C115" s="1" t="s">
@@ -7125,6 +7197,105 @@
       </c>
       <c r="K119" s="3"/>
       <c r="O119" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A120" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>761</v>
+      </c>
+      <c r="G120" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="J120" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="K120" s="3"/>
+      <c r="O120" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A121" s="7" t="s">
+        <v>756</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>762</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="J121" s="9" t="s">
+        <v>772</v>
+      </c>
+      <c r="K121" s="3"/>
+      <c r="O121" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A122" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>760</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F122" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="G122" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="J122" s="9" t="s">
+        <v>773</v>
+      </c>
+      <c r="K122" s="3"/>
+      <c r="O122" s="7" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
release the array test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
@@ -3055,8 +3055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5274,7 +5274,7 @@
         <v>376</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>602</v>
+        <v>8</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>378</v>
@@ -5310,7 +5310,7 @@
         <v>377</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>602</v>
+        <v>8</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>384</v>
@@ -5346,7 +5346,7 @@
         <v>390</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>602</v>
+        <v>8</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>391</v>
@@ -5382,7 +5382,7 @@
         <v>396</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>602</v>
+        <v>8</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>397</v>

</xml_diff>

<commit_message>
enable mysql preparedStatement batch insert case and add case about unix_timestamp(now()) as default value in table definition
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="783">
   <si>
     <t>TestID</t>
   </si>
@@ -2669,6 +2669,31 @@
   </si>
   <si>
     <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_024</t>
+  </si>
+  <si>
+    <t>字段默认值为当前时间的时间戳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_value20</t>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/insert_024.csv</t>
+  </si>
+  <si>
+    <t>select orderid,productname,char_length(ordertime) c_o from $schema33</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3053,10 +3078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O122"/>
+  <dimension ref="A1:O123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="E109" workbookViewId="0">
+      <selection activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7296,6 +7321,39 @@
       </c>
       <c r="K122" s="3"/>
       <c r="O122" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A123" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="J123" s="9" t="s">
+        <v>781</v>
+      </c>
+      <c r="K123" s="3"/>
+      <c r="O123" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add count query in hash partition table
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="790">
   <si>
     <t>TestID</t>
   </si>
@@ -2695,6 +2695,32 @@
   <si>
     <t>select orderid,productname,char_length(ordertime) c_o from $schema33</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_025</t>
+  </si>
+  <si>
+    <t>hash分区的表插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>partition50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value_partition50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,name,age,gmt,price,amount,address,birthday,create_time,update_time,zip_code,is_delete,feature,user_info,feature_id from $partition50 order by id limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/insert_025.csv</t>
   </si>
 </sst>
 </file>
@@ -2734,7 +2760,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2744,6 +2770,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2760,7 +2792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2777,6 +2809,7 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3078,10 +3111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O123"/>
+  <dimension ref="A1:O124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E109" workbookViewId="0">
-      <selection activeCell="J123" sqref="J123"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3645,7 +3678,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>102</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -5657,7 +5690,7 @@
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="12" t="s">
         <v>432</v>
       </c>
       <c r="B76" s="7" t="s">
@@ -5693,7 +5726,7 @@
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="12" t="s">
         <v>433</v>
       </c>
       <c r="B77" s="7" t="s">
@@ -5729,7 +5762,7 @@
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="12" t="s">
         <v>434</v>
       </c>
       <c r="B78" s="7" t="s">
@@ -5765,7 +5798,7 @@
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="12" t="s">
         <v>435</v>
       </c>
       <c r="B79" s="7" t="s">
@@ -5801,7 +5834,7 @@
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="12" t="s">
         <v>436</v>
       </c>
       <c r="B80" s="7" t="s">
@@ -5837,7 +5870,7 @@
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="12" t="s">
         <v>437</v>
       </c>
       <c r="B81" s="7" t="s">
@@ -5873,7 +5906,7 @@
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="12" t="s">
         <v>438</v>
       </c>
       <c r="B82" s="7" t="s">
@@ -5909,7 +5942,7 @@
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="12" t="s">
         <v>439</v>
       </c>
       <c r="B83" s="7" t="s">
@@ -5945,7 +5978,7 @@
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="12" t="s">
         <v>440</v>
       </c>
       <c r="B84" s="7" t="s">
@@ -5981,7 +6014,7 @@
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="12" t="s">
         <v>484</v>
       </c>
       <c r="B85" s="7" t="s">
@@ -6017,7 +6050,7 @@
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="12" t="s">
         <v>485</v>
       </c>
       <c r="B86" s="7" t="s">
@@ -6053,7 +6086,7 @@
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="12" t="s">
         <v>495</v>
       </c>
       <c r="B87" s="7" t="s">
@@ -6089,7 +6122,7 @@
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="12" t="s">
         <v>496</v>
       </c>
       <c r="B88" s="7" t="s">
@@ -6125,7 +6158,7 @@
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A89" s="11" t="s">
+      <c r="A89" s="12" t="s">
         <v>497</v>
       </c>
       <c r="B89" s="7" t="s">
@@ -6161,7 +6194,7 @@
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="12" t="s">
         <v>498</v>
       </c>
       <c r="B90" s="7" t="s">
@@ -6197,7 +6230,7 @@
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A91" s="11" t="s">
+      <c r="A91" s="12" t="s">
         <v>499</v>
       </c>
       <c r="B91" s="7" t="s">
@@ -6233,7 +6266,7 @@
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A92" s="11" t="s">
+      <c r="A92" s="12" t="s">
         <v>500</v>
       </c>
       <c r="B92" s="7" t="s">
@@ -6269,7 +6302,7 @@
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A93" s="11" t="s">
+      <c r="A93" s="12" t="s">
         <v>501</v>
       </c>
       <c r="B93" s="7" t="s">
@@ -6305,7 +6338,7 @@
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A94" s="11" t="s">
+      <c r="A94" s="12" t="s">
         <v>502</v>
       </c>
       <c r="B94" s="7" t="s">
@@ -6341,7 +6374,7 @@
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A95" s="11" t="s">
+      <c r="A95" s="12" t="s">
         <v>503</v>
       </c>
       <c r="B95" s="7" t="s">
@@ -6377,7 +6410,7 @@
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A96" s="11" t="s">
+      <c r="A96" s="12" t="s">
         <v>504</v>
       </c>
       <c r="B96" s="7" t="s">
@@ -6413,7 +6446,7 @@
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="12" t="s">
         <v>505</v>
       </c>
       <c r="B97" s="7" t="s">
@@ -6449,7 +6482,7 @@
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="12" t="s">
         <v>506</v>
       </c>
       <c r="B98" s="7" t="s">
@@ -6485,7 +6518,7 @@
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A99" s="11" t="s">
+      <c r="A99" s="12" t="s">
         <v>507</v>
       </c>
       <c r="B99" s="7" t="s">
@@ -6521,7 +6554,7 @@
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A100" s="11" t="s">
+      <c r="A100" s="12" t="s">
         <v>508</v>
       </c>
       <c r="B100" s="7" t="s">
@@ -6557,7 +6590,7 @@
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A101" s="11" t="s">
+      <c r="A101" s="12" t="s">
         <v>509</v>
       </c>
       <c r="B101" s="7" t="s">
@@ -6593,7 +6626,7 @@
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A102" s="11" t="s">
+      <c r="A102" s="12" t="s">
         <v>510</v>
       </c>
       <c r="B102" s="7" t="s">
@@ -6629,7 +6662,7 @@
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="12" t="s">
         <v>511</v>
       </c>
       <c r="B103" s="7" t="s">
@@ -6665,7 +6698,7 @@
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A104" s="11" t="s">
+      <c r="A104" s="12" t="s">
         <v>512</v>
       </c>
       <c r="B104" s="7" t="s">
@@ -6701,7 +6734,7 @@
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A105" s="11" t="s">
+      <c r="A105" s="12" t="s">
         <v>513</v>
       </c>
       <c r="B105" s="7" t="s">
@@ -6737,7 +6770,7 @@
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A106" s="11" t="s">
+      <c r="A106" s="12" t="s">
         <v>514</v>
       </c>
       <c r="B106" s="7" t="s">
@@ -6773,7 +6806,7 @@
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="12" t="s">
         <v>515</v>
       </c>
       <c r="B107" s="7" t="s">
@@ -6809,7 +6842,7 @@
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A108" s="11" t="s">
+      <c r="A108" s="12" t="s">
         <v>516</v>
       </c>
       <c r="B108" s="7" t="s">
@@ -6845,7 +6878,7 @@
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A109" s="11" t="s">
+      <c r="A109" s="12" t="s">
         <v>517</v>
       </c>
       <c r="B109" s="7" t="s">
@@ -6881,7 +6914,7 @@
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A110" s="11" t="s">
+      <c r="A110" s="12" t="s">
         <v>518</v>
       </c>
       <c r="B110" s="7" t="s">
@@ -6917,7 +6950,7 @@
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A111" s="11" t="s">
+      <c r="A111" s="12" t="s">
         <v>519</v>
       </c>
       <c r="B111" s="7" t="s">
@@ -6953,7 +6986,7 @@
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="12" t="s">
         <v>588</v>
       </c>
       <c r="B112" s="7" t="s">
@@ -6989,7 +7022,7 @@
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="12" t="s">
         <v>594</v>
       </c>
       <c r="B113" s="7" t="s">
@@ -7025,7 +7058,7 @@
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A114" s="11" t="s">
+      <c r="A114" s="12" t="s">
         <v>598</v>
       </c>
       <c r="B114" s="7" t="s">
@@ -7355,6 +7388,39 @@
       <c r="K123" s="3"/>
       <c r="O123" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A124" s="7" t="s">
+        <v>783</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D124" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="J124" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="K124" s="3"/>
+      <c r="O124" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update boolean test cases to support decimal
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/insert/sql_insert_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="812">
   <si>
     <t>TestID</t>
   </si>
@@ -2749,6 +2749,64 @@
   </si>
   <si>
     <t>array_04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_027</t>
+  </si>
+  <si>
+    <t>布尔型字段插入小数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert_value22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/insert_027.csv</t>
+  </si>
+  <si>
+    <t>布尔型数组插入元素为小数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array10_value58</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select in_use from $array10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/insert/expectedresult/complexdatatype/array/array_005.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array_05</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3133,10 +3191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O125"/>
+  <dimension ref="A1:O127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7475,6 +7533,75 @@
       </c>
       <c r="K125" s="3"/>
       <c r="O125" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A126" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="G126" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="J126" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="K126" s="3"/>
+      <c r="O126" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A127" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="D127" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="E127" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="J127" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="K127" s="3"/>
+      <c r="O127" s="7" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>